<commit_message>
Create account implemented in backend and tested
</commit_message>
<xml_diff>
--- a/Projekat - timetracking.xlsx
+++ b/Projekat - timetracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCH\Documents\MoneyTransferApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5BADB2-FBA1-4D66-9BD3-CF75423E9E21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A72C9AB-1681-4DC5-B3EA-D7E49CF6A2DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Naziv user storija</t>
   </si>
@@ -64,6 +64,36 @@
   </si>
   <si>
     <t>Proucavanje i setupovanje dockera</t>
+  </si>
+  <si>
+    <t>Kreiranje novcanika</t>
+  </si>
+  <si>
+    <t>Aplikativni sloj - Create account metoda</t>
+  </si>
+  <si>
+    <t>Bank service interface</t>
+  </si>
+  <si>
+    <t>Bank service mock</t>
+  </si>
+  <si>
+    <t>Test za kreiranje</t>
+  </si>
+  <si>
+    <t>15min</t>
+  </si>
+  <si>
+    <t>20min</t>
+  </si>
+  <si>
+    <t>45min</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>Frontend - Stranica za create account</t>
   </si>
 </sst>
 </file>
@@ -390,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="48.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
@@ -458,6 +488,60 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated timetracking and and bank service method name
</commit_message>
<xml_diff>
--- a/Projekat - timetracking.xlsx
+++ b/Projekat - timetracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCH\Documents\MoneyTransferApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A72C9AB-1681-4DC5-B3EA-D7E49CF6A2DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41835997-33D5-4ADA-8944-7D1F97462C2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Naziv user storija</t>
   </si>
@@ -93,7 +93,22 @@
     <t>30min</t>
   </si>
   <si>
-    <t>Frontend - Stranica za create account</t>
+    <t>1h 10min</t>
+  </si>
+  <si>
+    <t>1h 30min</t>
+  </si>
+  <si>
+    <t>1h 50min</t>
+  </si>
+  <si>
+    <t>Frontend - Stranica za create account *</t>
+  </si>
+  <si>
+    <t>Setup webappa *</t>
+  </si>
+  <si>
+    <t>*rad u losim uslovima</t>
   </si>
 </sst>
 </file>
@@ -420,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,12 +449,12 @@
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -450,12 +465,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -466,7 +484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -477,7 +495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -488,12 +506,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -504,12 +533,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -520,7 +555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -531,7 +566,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
SystemParameters and admin added
</commit_message>
<xml_diff>
--- a/Projekat - timetracking.xlsx
+++ b/Projekat - timetracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCH\Documents\MoneyTransferApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FDECD4-D780-4832-882B-156AA619276A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9AD3BF-BA4C-47EF-822A-BDF7C06C8AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
   <si>
     <t>Naziv user storija</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>Password change test</t>
+  </si>
+  <si>
+    <t>_____</t>
+  </si>
+  <si>
+    <t>____</t>
+  </si>
+  <si>
+    <t>New System parameters + admin</t>
   </si>
 </sst>
 </file>
@@ -534,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,6 +577,9 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" t="s">
         <v>27</v>
       </c>
@@ -620,6 +632,9 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -680,6 +695,9 @@
       <c r="A14" t="s">
         <v>30</v>
       </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -762,6 +780,9 @@
       <c r="A22" t="s">
         <v>40</v>
       </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -822,6 +843,9 @@
       <c r="A28" t="s">
         <v>46</v>
       </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -860,6 +884,9 @@
       <c r="A32" t="s">
         <v>50</v>
       </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -920,6 +947,9 @@
       <c r="A38" t="s">
         <v>57</v>
       </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -952,6 +982,22 @@
       </c>
       <c r="D41" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added admin service tests and timetracking updated
</commit_message>
<xml_diff>
--- a/Projekat - timetracking.xlsx
+++ b/Projekat - timetracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCH\Documents\MoneyTransferApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B2E5A7-9114-4381-85D1-BA0FB2FB9DF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72997345-BA85-4E39-AB93-581FBACB7342}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="74">
   <si>
     <t>Naziv user storija</t>
   </si>
@@ -240,7 +240,13 @@
     <t>adminservice tests</t>
   </si>
   <si>
-    <t>frontend</t>
+    <t>1h 15min</t>
+  </si>
+  <si>
+    <t>frontend - admin verify, block, unblock</t>
+  </si>
+  <si>
+    <t>frontend - parameter edit</t>
   </si>
 </sst>
 </file>
@@ -567,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,10 +1094,27 @@
       <c r="B50" t="s">
         <v>70</v>
       </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>